<commit_message>
Tweede ronde experimentatie af en opschoning main
</commit_message>
<xml_diff>
--- a/experiments/simulated annealing/Tabelresultaten.xlsx
+++ b/experiments/simulated annealing/Tabelresultaten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesv\Documents\RailNLProject\Team-Trein\experimentatie resultaten\simulated annealing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesv\Documents\RailNLProject\Team-Trein\experiments\simulated annealing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD68689-CFEB-432F-89E7-52BD9A6410BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E656CCE-08EC-4DE6-B701-AC27E079B4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A41B608-95EF-42B6-8E2B-7EC8DAE4784E}"/>
+    <workbookView xWindow="2196" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{6A41B608-95EF-42B6-8E2B-7EC8DAE4784E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelresultaten" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>0.4</t>
   </si>
@@ -99,6 +99,51 @@
   </si>
   <si>
     <t>6803.92</t>
+  </si>
+  <si>
+    <t>0.4125</t>
+  </si>
+  <si>
+    <t>0.425</t>
+  </si>
+  <si>
+    <t>0.4375</t>
+  </si>
+  <si>
+    <t>6810.28</t>
+  </si>
+  <si>
+    <t>6804.92</t>
+  </si>
+  <si>
+    <t>6762.28</t>
+  </si>
+  <si>
+    <t>6799.84</t>
+  </si>
+  <si>
+    <t>6802.28</t>
+  </si>
+  <si>
+    <t>6792.92</t>
+  </si>
+  <si>
+    <t>6835.92</t>
+  </si>
+  <si>
+    <t>6816.20</t>
+  </si>
+  <si>
+    <t>6822.28</t>
+  </si>
+  <si>
+    <t>6830.92</t>
+  </si>
+  <si>
+    <t>6817.92</t>
+  </si>
+  <si>
+    <t>6785.56</t>
   </si>
 </sst>
 </file>
@@ -502,15 +547,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57366105-2A13-43F9-B4E9-1AA1C2AA33BE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -526,8 +571,23 @@
       <c r="E1" s="1">
         <v>2000</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
+        <v>600</v>
+      </c>
+      <c r="I1" s="1">
+        <v>700</v>
+      </c>
+      <c r="J1" s="1">
+        <v>800</v>
+      </c>
+      <c r="K1" s="1">
+        <v>900</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -543,8 +603,23 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -560,8 +635,23 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -577,8 +667,23 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>